<commit_message>
change masterData file for import of products
</commit_message>
<xml_diff>
--- a/public/Master data.xlsx
+++ b/public/Master data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Wapi Univercity\Logistics\Docs for new clients\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{14083B45-C797-4AA8-A8ED-DB12DE27934A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{24EE2AE9-011C-4C1D-B8B7-5A431983B295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="27810" windowHeight="14025" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="27810" windowHeight="14025" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TO BE FILLED" sheetId="1" r:id="rId1"/>
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="108">
   <si>
     <t>PRODUCT IN PRIMARY/INNER/SALES PACKAGE</t>
   </si>
@@ -181,7 +181,7 @@
     <t>Special delivery/storage requests?</t>
   </si>
   <si>
-    <t>Purchase value, eur</t>
+    <t>Purchase value, per unit, eur</t>
   </si>
   <si>
     <t>Insurance?</t>
@@ -200,9 +200,6 @@
   </si>
   <si>
     <t>Expiration date, month?</t>
-  </si>
-  <si>
-    <t>Purchase value, per unit, eur</t>
   </si>
   <si>
     <t>The trade or marketing product name that you will see in the system. It should be short - up to 40 characters, but the less the better!</t>
@@ -1361,9 +1358,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD1000"/>
   <sheetViews>
-    <sheetView topLeftCell="S1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AB1" sqref="AB1:AB1048576"/>
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="T3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="15"/>
@@ -1437,7 +1434,7 @@
       <c r="AC1" s="19"/>
       <c r="AD1" s="12"/>
     </row>
-    <row r="2" spans="1:30" ht="45">
+    <row r="2" spans="1:30" ht="45.75">
       <c r="A2" s="38" t="s">
         <v>2</v>
       </c>
@@ -33528,7 +33525,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AD100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="111" zoomScaleNormal="111" workbookViewId="0">
+    <sheetView topLeftCell="T1" zoomScale="111" zoomScaleNormal="111" workbookViewId="0">
       <selection activeCell="Z2" sqref="Z2"/>
     </sheetView>
   </sheetViews>
@@ -33679,7 +33676,7 @@
         <v>25</v>
       </c>
       <c r="Z2" s="25" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="AA2" s="26" t="s">
         <v>27</v>
@@ -33696,201 +33693,201 @@
     </row>
     <row r="3" spans="1:30" s="4" customFormat="1" ht="189" customHeight="1">
       <c r="A3" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="C3" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="D3" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="E3" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="F3" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="17" t="s">
-        <v>39</v>
-      </c>
       <c r="G3" s="27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H3" s="101" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I3" s="101"/>
       <c r="J3" s="101"/>
       <c r="K3" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="L3" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="L3" s="16" t="s">
-        <v>42</v>
-      </c>
       <c r="M3" s="101" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N3" s="101"/>
       <c r="O3" s="101"/>
       <c r="P3" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q3" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="Q3" s="21" t="s">
+      <c r="R3" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="R3" s="21" t="s">
+      <c r="S3" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="S3" s="21" t="s">
+      <c r="T3" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="T3" s="27" t="s">
+      <c r="U3" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="U3" s="27" t="s">
+      <c r="V3" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="V3" s="17" t="s">
+      <c r="W3" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="X3" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y3" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="W3" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="X3" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y3" s="21" t="s">
+      <c r="Z3" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="Z3" s="16" t="s">
+      <c r="AA3" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="AA3" s="21" t="s">
+      <c r="AB3" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="AB3" s="16" t="s">
+      <c r="AC3" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="AC3" s="27" t="s">
+      <c r="AD3" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="AD3" s="17" t="s">
+    </row>
+    <row r="4" spans="1:30" s="3" customFormat="1" ht="39.75" customHeight="1">
+      <c r="A4" s="14" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="4" spans="1:30" s="3" customFormat="1" ht="39.75" customHeight="1">
-      <c r="A4" s="14" t="s">
+      <c r="B4" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="F4" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="H4" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="K4" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="L4" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="M4" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="N4" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="O4" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="P4" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q4" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="R4" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="S4" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="T4" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="F4" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="G4" s="22" t="s">
+      <c r="U4" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="H4" s="14" t="s">
-        <v>56</v>
+      <c r="V4" s="14" t="s">
+        <v>55</v>
       </c>
-      <c r="I4" s="14" t="s">
-        <v>56</v>
+      <c r="W4" s="14" t="s">
+        <v>55</v>
       </c>
-      <c r="J4" s="14" t="s">
-        <v>56</v>
+      <c r="X4" s="14" t="s">
+        <v>55</v>
       </c>
-      <c r="K4" s="14" t="s">
-        <v>56</v>
+      <c r="Y4" s="29" t="s">
+        <v>57</v>
       </c>
-      <c r="L4" s="14" t="s">
-        <v>56</v>
+      <c r="Z4" s="94" t="s">
+        <v>55</v>
       </c>
-      <c r="M4" s="14" t="s">
-        <v>56</v>
+      <c r="AA4" s="29" t="s">
+        <v>57</v>
       </c>
-      <c r="N4" s="14" t="s">
-        <v>56</v>
+      <c r="AB4" s="94" t="s">
+        <v>55</v>
       </c>
-      <c r="O4" s="14" t="s">
-        <v>56</v>
+      <c r="AC4" s="29" t="s">
+        <v>57</v>
       </c>
-      <c r="P4" s="14" t="s">
-        <v>56</v>
+      <c r="AD4" s="14" t="s">
+        <v>55</v>
       </c>
-      <c r="Q4" s="33" t="s">
+    </row>
+    <row r="5" spans="1:30">
+      <c r="A5" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="R4" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="S4" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="T4" s="34" t="s">
-        <v>58</v>
-      </c>
-      <c r="U4" s="34" t="s">
-        <v>58</v>
-      </c>
-      <c r="V4" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="W4" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="X4" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y4" s="29" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z4" s="94" t="s">
-        <v>56</v>
-      </c>
-      <c r="AA4" s="29" t="s">
-        <v>58</v>
-      </c>
-      <c r="AB4" s="94" t="s">
-        <v>56</v>
-      </c>
-      <c r="AC4" s="29" t="s">
-        <v>58</v>
-      </c>
-      <c r="AD4" s="14" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:30">
-      <c r="A5" s="15" t="s">
+      <c r="B5" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="C5" s="15" t="s">
         <v>60</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>61</v>
       </c>
       <c r="D5" s="18">
         <v>35415741145</v>
       </c>
       <c r="E5" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="G5" s="28" t="s">
         <v>63</v>
-      </c>
-      <c r="G5" s="28" t="s">
-        <v>64</v>
       </c>
       <c r="H5" s="15">
         <v>120</v>
@@ -33905,7 +33902,7 @@
         <v>5</v>
       </c>
       <c r="L5" s="18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M5" s="15">
         <v>130</v>
@@ -33917,57 +33914,57 @@
         <v>260</v>
       </c>
       <c r="P5" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q5" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="Q5" s="28" t="s">
+      <c r="R5" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="R5" s="28" t="s">
+      <c r="S5" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="S5" s="28" t="s">
+      <c r="T5" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="T5" s="28" t="s">
+      <c r="U5" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="U5" s="23" t="s">
+      <c r="V5" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="V5" s="15" t="s">
+      <c r="W5" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="W5" s="15" t="s">
-        <v>73</v>
-      </c>
       <c r="X5" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Y5" s="30" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Z5" s="15">
         <v>10</v>
       </c>
       <c r="AA5" s="28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AB5" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AC5" s="31">
         <v>6461316843811</v>
       </c>
       <c r="AD5" s="15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" ht="18" customHeight="1">
+      <c r="A6" s="15" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="6" spans="1:30" ht="18" customHeight="1">
-      <c r="A6" s="15" t="s">
+      <c r="B6" s="15" t="s">
         <v>77</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>78</v>
       </c>
       <c r="C6" s="15">
         <v>61151351</v>
@@ -33976,13 +33973,13 @@
         <v>12531515352</v>
       </c>
       <c r="E6" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="F6" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="G6" s="28" t="s">
         <v>80</v>
-      </c>
-      <c r="G6" s="28" t="s">
-        <v>81</v>
       </c>
       <c r="H6" s="15">
         <v>200</v>
@@ -33997,7 +33994,7 @@
         <v>10</v>
       </c>
       <c r="L6" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M6" s="15">
         <v>210</v>
@@ -34009,70 +34006,70 @@
         <v>1210</v>
       </c>
       <c r="P6" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q6" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="Q6" s="28" t="s">
+      <c r="R6" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="S6" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="T6" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="U6" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="V6" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="W6" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="X6" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y6" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z6" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="R6" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="S6" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="T6" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="U6" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="V6" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="W6" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="X6" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="Y6" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="Z6" s="15" t="s">
-        <v>85</v>
-      </c>
       <c r="AA6" s="28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AB6" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AC6" s="31">
         <v>6461316843811</v>
       </c>
       <c r="AD6" s="15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30">
+      <c r="A7" s="15" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="7" spans="1:30">
-      <c r="A7" s="15" t="s">
+      <c r="B7" s="15" t="s">
         <v>88</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>89</v>
       </c>
       <c r="C7" s="15">
         <v>46318</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E7" s="23"/>
       <c r="F7" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G7" s="28" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H7" s="15">
         <v>200</v>
@@ -34087,7 +34084,7 @@
         <v>1</v>
       </c>
       <c r="L7" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M7" s="15">
         <v>200</v>
@@ -34099,49 +34096,49 @@
         <v>120</v>
       </c>
       <c r="P7" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q7" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="Q7" s="28" t="s">
+      <c r="R7" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="S7" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="T7" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="U7" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="V7" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="W7" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="X7" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y7" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z7" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="R7" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="S7" s="28" t="s">
-        <v>92</v>
-      </c>
-      <c r="T7" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="U7" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="V7" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="W7" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="X7" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="Y7" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="Z7" s="15" t="s">
-        <v>85</v>
-      </c>
       <c r="AA7" s="28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AB7" s="15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AC7" s="31">
         <v>6461316843811</v>
       </c>
       <c r="AD7" s="15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:30">
@@ -37147,22 +37144,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>98</v>
-      </c>
-    </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -37182,12 +37179,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -37215,22 +37212,22 @@
     </row>
     <row r="4" spans="3:3">
       <c r="C4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="3:3">
+      <c r="C5" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="3:3">
-      <c r="C5" t="s">
+    <row r="6" spans="3:3">
+      <c r="C6" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="3:3">
-      <c r="C6" t="s">
-        <v>102</v>
-      </c>
-    </row>
     <row r="7" spans="3:3">
       <c r="C7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -37254,17 +37251,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>105</v>
-      </c>
-    </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -37284,12 +37281,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -37298,14 +37295,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9695963a-867a-4dc9-a585-16d77b89968a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="30fa0888-ff81-4143-a4c4-8008035dd0ee" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -37546,16 +37541,18 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9695963a-867a-4dc9-a585-16d77b89968a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="30fa0888-ff81-4143-a4c4-8008035dd0ee" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0357A2A7-6D61-4DD4-AF1F-01EE3FF28186}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9E268F1-04F1-424C-9BD1-724E14C6D65A}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -37563,5 +37560,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9E268F1-04F1-424C-9BD1-724E14C6D65A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0357A2A7-6D61-4DD4-AF1F-01EE3FF28186}"/>
 </file>
</xml_diff>

<commit_message>
add new MasterData template (added text about Additional Virtual product)
</commit_message>
<xml_diff>
--- a/public/Master data.xlsx
+++ b/public/Master data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28412"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Wapi Univercity\Logistics\Docs for new clients\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sancha/Documents/WAPI/Wapi/Работа/Переход на 1С/UI/Master data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{24EE2AE9-011C-4C1D-B8B7-5A431983B295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{84483ADF-95EB-4346-8F6F-7E82B470640C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="27810" windowHeight="14025" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="400" yWindow="760" windowWidth="27820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TO BE FILLED" sheetId="1" r:id="rId1"/>
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="109">
   <si>
     <t>PRODUCT IN PRIMARY/INNER/SALES PACKAGE</t>
   </si>
@@ -197,6 +197,9 @@
   </si>
   <si>
     <t>*PLEASE FILL IN "TO BE FILLED" SHEET, NOT THIS EXAMPLE SHEET</t>
+  </si>
+  <si>
+    <t>ADDITIONAL VIRTUAL PRODUCT MUST BE CREATED MANUALLY (CLICK ON "ADD PRODUCT" BUTTON IN UI, SELECT "ADDITIONAL VIRTUAL PRODUCT" IN THE CHECKBOX)</t>
   </si>
   <si>
     <t>Expiration date, month?</t>
@@ -671,7 +674,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -926,6 +929,9 @@
     <xf numFmtId="2" fontId="19" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1358,8 +1364,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="T3" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>
@@ -1404,20 +1410,20 @@
       <c r="C1" s="12"/>
       <c r="D1" s="12"/>
       <c r="E1" s="19"/>
-      <c r="F1" s="97" t="s">
+      <c r="F1" s="98" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="97"/>
-      <c r="H1" s="97"/>
-      <c r="I1" s="97"/>
-      <c r="J1" s="97"/>
-      <c r="K1" s="98" t="s">
+      <c r="G1" s="98"/>
+      <c r="H1" s="98"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="99" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="98"/>
-      <c r="M1" s="98"/>
-      <c r="N1" s="98"/>
-      <c r="O1" s="98"/>
+      <c r="L1" s="99"/>
+      <c r="M1" s="99"/>
+      <c r="N1" s="99"/>
+      <c r="O1" s="99"/>
       <c r="P1" s="91"/>
       <c r="Q1" s="19"/>
       <c r="R1" s="19"/>
@@ -1434,7 +1440,7 @@
       <c r="AC1" s="19"/>
       <c r="AD1" s="12"/>
     </row>
-    <row r="2" spans="1:30" ht="45.75">
+    <row r="2" spans="1:30" ht="48">
       <c r="A2" s="38" t="s">
         <v>2</v>
       </c>
@@ -33525,11 +33531,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AD100"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" zoomScale="111" zoomScaleNormal="111" workbookViewId="0">
-      <selection activeCell="Z2" sqref="Z2"/>
+    <sheetView zoomScale="111" zoomScaleNormal="111" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="18.95"/>
   <cols>
     <col min="1" max="1" width="23.69921875" style="11" customWidth="1"/>
     <col min="2" max="2" width="31.8984375" style="11" customWidth="1"/>
@@ -33561,28 +33567,30 @@
     <col min="30" max="30" width="28.296875" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="1" customFormat="1" ht="42.95" customHeight="1">
-      <c r="A1" s="92" t="s">
+    <row r="1" spans="1:30" s="1" customFormat="1" ht="81" customHeight="1">
+      <c r="A1" s="97" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="12"/>
+      <c r="B1" s="92" t="s">
+        <v>32</v>
+      </c>
       <c r="C1" s="12"/>
       <c r="D1" s="12"/>
       <c r="E1" s="19"/>
-      <c r="F1" s="99" t="s">
+      <c r="F1" s="100" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="99"/>
-      <c r="H1" s="99"/>
-      <c r="I1" s="99"/>
-      <c r="J1" s="99"/>
-      <c r="K1" s="100" t="s">
+      <c r="G1" s="100"/>
+      <c r="H1" s="100"/>
+      <c r="I1" s="100"/>
+      <c r="J1" s="100"/>
+      <c r="K1" s="101" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="100"/>
-      <c r="M1" s="100"/>
-      <c r="N1" s="100"/>
-      <c r="O1" s="100"/>
+      <c r="L1" s="101"/>
+      <c r="M1" s="101"/>
+      <c r="N1" s="101"/>
+      <c r="O1" s="101"/>
       <c r="P1" s="91"/>
       <c r="Q1" s="19"/>
       <c r="R1" s="19"/>
@@ -33658,7 +33666,7 @@
         <v>19</v>
       </c>
       <c r="T2" s="26" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="U2" s="26" t="s">
         <v>21</v>
@@ -33693,201 +33701,201 @@
     </row>
     <row r="3" spans="1:30" s="4" customFormat="1" ht="189" customHeight="1">
       <c r="A3" s="16" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G3" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="H3" s="101" t="s">
         <v>39</v>
       </c>
-      <c r="I3" s="101"/>
-      <c r="J3" s="101"/>
-      <c r="K3" s="16" t="s">
+      <c r="H3" s="102" t="s">
         <v>40</v>
       </c>
-      <c r="L3" s="16" t="s">
+      <c r="I3" s="102"/>
+      <c r="J3" s="102"/>
+      <c r="K3" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="M3" s="101" t="s">
-        <v>39</v>
-      </c>
-      <c r="N3" s="101"/>
-      <c r="O3" s="101"/>
-      <c r="P3" s="16" t="s">
+      <c r="L3" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="Q3" s="21" t="s">
+      <c r="M3" s="102" t="s">
+        <v>40</v>
+      </c>
+      <c r="N3" s="102"/>
+      <c r="O3" s="102"/>
+      <c r="P3" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="R3" s="21" t="s">
+      <c r="Q3" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="S3" s="21" t="s">
+      <c r="R3" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="T3" s="27" t="s">
+      <c r="S3" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="U3" s="27" t="s">
+      <c r="T3" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="V3" s="17" t="s">
+      <c r="U3" s="27" t="s">
         <v>48</v>
       </c>
+      <c r="V3" s="17" t="s">
+        <v>49</v>
+      </c>
       <c r="W3" s="17" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="X3" s="17" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="Y3" s="21" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="Z3" s="16" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="AA3" s="21" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AB3" s="16" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="AC3" s="27" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="AD3" s="17" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:30" s="3" customFormat="1" ht="39.75" customHeight="1">
       <c r="A4" s="14" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E4" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="F4" s="14" t="s">
-        <v>55</v>
+      <c r="G4" s="22" t="s">
+        <v>57</v>
       </c>
-      <c r="G4" s="22" t="s">
+      <c r="H4" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="H4" s="14" t="s">
-        <v>55</v>
-      </c>
       <c r="I4" s="14" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="K4" s="14" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L4" s="14" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="M4" s="14" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="N4" s="14" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="O4" s="14" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="P4" s="14" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="Q4" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="R4" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="R4" s="33" t="s">
+      <c r="S4" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="T4" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="U4" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="V4" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="S4" s="33" t="s">
+      <c r="W4" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="T4" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="U4" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="V4" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="W4" s="14" t="s">
-        <v>55</v>
-      </c>
       <c r="X4" s="14" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="Y4" s="29" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="Z4" s="94" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AA4" s="29" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AB4" s="94" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AC4" s="29" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AD4" s="14" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:30">
       <c r="A5" s="15" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D5" s="18">
         <v>35415741145</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G5" s="28" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H5" s="15">
         <v>120</v>
@@ -33902,7 +33910,7 @@
         <v>5</v>
       </c>
       <c r="L5" s="18" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="M5" s="15">
         <v>130</v>
@@ -33914,57 +33922,57 @@
         <v>260</v>
       </c>
       <c r="P5" s="15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q5" s="28" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="R5" s="28" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="S5" s="28" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="T5" s="28" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="U5" s="23" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="V5" s="15" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="W5" s="15" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="X5" s="15" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Y5" s="30" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="Z5" s="15">
         <v>10</v>
       </c>
       <c r="AA5" s="28" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AB5" s="15" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AC5" s="31">
         <v>6461316843811</v>
       </c>
       <c r="AD5" s="15" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:30" ht="18" customHeight="1">
       <c r="A6" s="15" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C6" s="15">
         <v>61151351</v>
@@ -33973,13 +33981,13 @@
         <v>12531515352</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G6" s="28" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H6" s="15">
         <v>200</v>
@@ -33994,7 +34002,7 @@
         <v>10</v>
       </c>
       <c r="L6" s="15" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="M6" s="15">
         <v>210</v>
@@ -34006,70 +34014,70 @@
         <v>1210</v>
       </c>
       <c r="P6" s="15" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="Q6" s="28" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="R6" s="28" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="S6" s="28" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="T6" s="28" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="U6" s="23" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="V6" s="15" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="W6" s="15" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="X6" s="15" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Y6" s="28" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Z6" s="15" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="AA6" s="28" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AB6" s="15" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="AC6" s="31">
         <v>6461316843811</v>
       </c>
       <c r="AD6" s="15" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:30">
       <c r="A7" s="15" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C7" s="15">
         <v>46318</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E7" s="23"/>
       <c r="F7" s="15" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G7" s="28" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H7" s="15">
         <v>200</v>
@@ -34084,7 +34092,7 @@
         <v>1</v>
       </c>
       <c r="L7" s="15" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="M7" s="15">
         <v>200</v>
@@ -34096,49 +34104,49 @@
         <v>120</v>
       </c>
       <c r="P7" s="15" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="Q7" s="28" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="R7" s="28" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="S7" s="28" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="T7" s="28" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="U7" s="23" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="V7" s="15" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="W7" s="15" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="X7" s="15" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Y7" s="28" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Z7" s="15" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="AA7" s="28" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AB7" s="15" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AC7" s="31">
         <v>6461316843811</v>
       </c>
       <c r="AD7" s="15" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:30">
@@ -37137,29 +37145,29 @@
       <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.09765625" defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultColWidth="11.09765625" defaultRowHeight="18.95"/>
   <cols>
     <col min="1" max="1" width="36.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -37175,16 +37183,16 @@
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.09765625" defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultColWidth="11.09765625" defaultRowHeight="18.95"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -37200,34 +37208,34 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="18.95"/>
   <cols>
     <col min="3" max="3" width="22.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:3" ht="37.5">
+    <row r="3" spans="3:3" ht="39.950000000000003">
       <c r="C3" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="3:3">
       <c r="C4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="3:3">
       <c r="C5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="3:3">
       <c r="C6" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="3:3">
       <c r="C7" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -37244,24 +37252,24 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.09765625" defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultColWidth="11.09765625" defaultRowHeight="18.95"/>
   <cols>
     <col min="1" max="1" width="25.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -37277,16 +37285,16 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.09765625" defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultColWidth="11.09765625" defaultRowHeight="18.95"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -37295,6 +37303,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="61fb5273-9fa9-47b1-aee4-88cf85ecd011">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b81398df-9a3a-473d-8e44-cc5041003447" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -37303,11 +37322,11 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100EC88CE037167F34FA74CD27748A71530" ma:contentTypeVersion="15" ma:contentTypeDescription="Loo uus dokument" ma:contentTypeScope="" ma:versionID="15b7a78525e1b8faae5c721de09d913e">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9695963a-867a-4dc9-a585-16d77b89968a" xmlns:ns3="30fa0888-ff81-4143-a4c4-8008035dd0ee" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1a2ff22316554286429b35252e12342a" ns2:_="" ns3:_="">
-    <xsd:import namespace="9695963a-867a-4dc9-a585-16d77b89968a"/>
-    <xsd:import namespace="30fa0888-ff81-4143-a4c4-8008035dd0ee"/>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004E609D4606550E41B3933AD7C596A883" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="18280195e7def4d54b236bc0479c09ba">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="61fb5273-9fa9-47b1-aee4-88cf85ecd011" xmlns:ns3="b81398df-9a3a-473d-8e44-cc5041003447" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0bed23160e317b0cfacc9864bed1c970" ns2:_="" ns3:_="">
+    <xsd:import namespace="61fb5273-9fa9-47b1-aee4-88cf85ecd011"/>
+    <xsd:import namespace="b81398df-9a3a-473d-8e44-cc5041003447"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
@@ -37316,18 +37335,15 @@
               <xsd:all>
                 <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
-                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
-                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -37335,7 +37351,7 @@
       </xsd:complexType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="9695963a-867a-4dc9-a585-16d77b89968a" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="61fb5273-9fa9-47b1-aee4-88cf85ecd011" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
@@ -37348,88 +37364,55 @@
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="10" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+    <xsd:element name="MediaServiceSearchProperties" ma:index="10" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="11" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceAutoTags" ma:index="11" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="b9506e52-7e6f-4938-8c0d-0e8b16a3f561" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="15" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="12" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+    <xsd:element name="MediaServiceOCR" ma:index="16" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="13" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+    <xsd:element name="MediaServiceGenerationTime" ma:index="17" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="14" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+    <xsd:element name="MediaServiceEventHashCode" ma:index="18" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="15" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceKeyPoints" ma:index="16" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaLengthInSeconds" ma:index="17" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+    <xsd:element name="MediaLengthInSeconds" ma:index="19" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="21" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Pildisildid" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="b9506e52-7e6f-4938-8c0d-0e8b16a3f561" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="30fa0888-ff81-4143-a4c4-8008035dd0ee" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="b81398df-9a3a-473d-8e44-cc5041003447" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="18" nillable="true" ma:displayName="Ühiskasutuses" ma:internalName="SharedWithUsers" ma:readOnly="true">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:UserMulti">
-            <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="19" nillable="true" ma:displayName="Ühiskasutusse andmise üksikasjad" ma:internalName="SharedWithDetails" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TaxCatchAll" ma:index="22" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{4b06c8dd-666a-4039-8b8a-50e2ba7c8212}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="30fa0888-ff81-4143-a4c4-8008035dd0ee">
+    <xsd:element name="TaxCatchAll" ma:index="14" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{efc9519b-137d-4e74-9f75-e409a3d4d103}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="b81398df-9a3a-473d-8e44-cc5041003447">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:MultiChoiceLookup">
@@ -37450,8 +37433,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Sisutüüp"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Pealkiri"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -37540,25 +37523,14 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9695963a-867a-4dc9-a585-16d77b89968a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="30fa0888-ff81-4143-a4c4-8008035dd0ee" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0357A2A7-6D61-4DD4-AF1F-01EE3FF28186}"/>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9E268F1-04F1-424C-9BD1-724E14C6D65A}"/>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70ECC47C-9C4F-4F26-B4BB-4308F37DF5A5}"/>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0357A2A7-6D61-4DD4-AF1F-01EE3FF28186}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5610BAD4-CFB6-4EF0-B295-1BD4010D6909}"/>
 </file>
</xml_diff>